<commit_message>
CareConnect IG Mock up
</commit_message>
<xml_diff>
--- a/docs/CareConnect-Encounter-1.xlsx
+++ b/docs/CareConnect-Encounter-1.xlsx
@@ -2475,16 +2475,16 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="68.078125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="29.36328125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="29.359375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.6953125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.62109375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.7421875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="125.1875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="125.18359375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -2495,19 +2495,19 @@
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
     <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.07421875" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="143.5625" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="68.71875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.6875" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="19.7265625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.0390625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="44.98828125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="31" max="31" width="44.984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.21484375" customWidth="true" bestFit="true"/>
+    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Added in HL7 UK FHIR Resources
</commit_message>
<xml_diff>
--- a/docs/CareConnect-Encounter-1.xlsx
+++ b/docs/CareConnect-Encounter-1.xlsx
@@ -2475,16 +2475,16 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="68.078125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="29.36328125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="29.359375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.6953125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.62109375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.7421875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="125.1875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="125.18359375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -2495,19 +2495,19 @@
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
     <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.07421875" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="143.5625" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="68.71875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.6875" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="19.7265625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.0390625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="44.98828125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="31" max="31" width="44.984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.21484375" customWidth="true" bestFit="true"/>
+    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
   </cols>
   <sheetData>

</xml_diff>